<commit_message>
added vix and move to pca mastersheet
</commit_message>
<xml_diff>
--- a/data/PCA Mastersheet.xlsx
+++ b/data/PCA Mastersheet.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianyishen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aliceye/Desktop/CryptoMacroecon-Prediction-CSUREMM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A26D3D1D-7B4F-F54F-8982-4C7974AA65B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45D69DA9-17AF-964B-B0A6-308A5F490996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8500" yWindow="760" windowWidth="20900" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Tether</t>
   </si>
@@ -42,6 +55,12 @@
   <si>
     <t>Month</t>
   </si>
+  <si>
+    <t>VIX</t>
+  </si>
+  <si>
+    <t>MOVE</t>
+  </si>
 </sst>
 </file>
 
@@ -50,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +81,19 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -100,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -108,6 +140,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,15 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -440,8 +474,14 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42979</v>
       </c>
@@ -454,8 +494,14 @@
       <c r="D2">
         <v>-3.8283</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="4">
+        <v>10.59</v>
+      </c>
+      <c r="I2" s="4">
+        <v>52.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43009</v>
       </c>
@@ -468,8 +514,14 @@
       <c r="D3">
         <v>-3.73861</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="4">
+        <v>9.51</v>
+      </c>
+      <c r="I3" s="4">
+        <v>51.15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43040</v>
       </c>
@@ -482,8 +534,14 @@
       <c r="D4">
         <v>-4.0195100000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="4">
+        <v>10.18</v>
+      </c>
+      <c r="I4" s="4">
+        <v>46.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43070</v>
       </c>
@@ -496,8 +554,14 @@
       <c r="D5">
         <v>-2.55687</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="4">
+        <v>11.28</v>
+      </c>
+      <c r="I5" s="4">
+        <v>46.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43101</v>
       </c>
@@ -510,8 +574,14 @@
       <c r="D6">
         <v>-2.7519300000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="4">
+        <v>11.04</v>
+      </c>
+      <c r="I6" s="4">
+        <v>57.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43132</v>
       </c>
@@ -530,8 +600,14 @@
       <c r="G7">
         <v>0.69513919930678969</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="4">
+        <v>13.54</v>
+      </c>
+      <c r="I7" s="4">
+        <v>62.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43160</v>
       </c>
@@ -550,8 +626,14 @@
       <c r="G8">
         <v>0.63927494473862989</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="4">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="I8" s="4">
+        <v>58.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43191</v>
       </c>
@@ -570,8 +652,14 @@
       <c r="G9">
         <v>0.50098847876597907</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="4">
+        <v>19.97</v>
+      </c>
+      <c r="I9" s="4">
+        <v>50.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43221</v>
       </c>
@@ -590,8 +678,14 @@
       <c r="G10">
         <v>0.66696769061145011</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="4">
+        <v>15.93</v>
+      </c>
+      <c r="I10" s="4">
+        <v>60.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43252</v>
       </c>
@@ -610,8 +704,14 @@
       <c r="G11">
         <v>0.75985697200250979</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="4">
+        <v>15.43</v>
+      </c>
+      <c r="I11" s="4">
+        <v>51.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43282</v>
       </c>
@@ -630,8 +730,14 @@
       <c r="G12">
         <v>0.7351609440187733</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="4">
+        <v>16.09</v>
+      </c>
+      <c r="I12" s="4">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43313</v>
       </c>
@@ -650,8 +756,14 @@
       <c r="G13">
         <v>1.222581111621023</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="4">
+        <v>12.83</v>
+      </c>
+      <c r="I13" s="4">
+        <v>50.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43344</v>
       </c>
@@ -670,8 +782,14 @@
       <c r="G14">
         <v>1.21168818638352</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="4">
+        <v>12.86</v>
+      </c>
+      <c r="I14" s="4">
+        <v>46.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43374</v>
       </c>
@@ -690,8 +808,14 @@
       <c r="G15">
         <v>1.0412906797666159</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="4">
+        <v>12.12</v>
+      </c>
+      <c r="I15" s="4">
+        <v>60.13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43405</v>
       </c>
@@ -710,8 +834,14 @@
       <c r="G16">
         <v>1.1622393564132669</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="4">
+        <v>21.23</v>
+      </c>
+      <c r="I16" s="4">
+        <v>52.43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43435</v>
       </c>
@@ -730,8 +860,14 @@
       <c r="G17">
         <v>0.36142586409146982</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="4">
+        <v>18.07</v>
+      </c>
+      <c r="I17" s="4">
+        <v>66.58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43466</v>
       </c>
@@ -753,8 +889,14 @@
       <c r="G18">
         <v>0.27953866868116672</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="4">
+        <v>25.42</v>
+      </c>
+      <c r="I18" s="4">
+        <v>49.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43497</v>
       </c>
@@ -776,8 +918,14 @@
       <c r="G19">
         <v>0.14064436052754969</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="4">
+        <v>16.57</v>
+      </c>
+      <c r="I19" s="4">
+        <v>47.22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43525</v>
       </c>
@@ -799,8 +947,14 @@
       <c r="G20">
         <v>0.32423672889485822</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="4">
+        <v>14.78</v>
+      </c>
+      <c r="I20" s="4">
+        <v>58.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43556</v>
       </c>
@@ -822,8 +976,14 @@
       <c r="G21">
         <v>0.46782093003803282</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="4">
+        <v>13.71</v>
+      </c>
+      <c r="I21" s="4">
+        <v>49.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43586</v>
       </c>
@@ -845,8 +1005,14 @@
       <c r="G22">
         <v>0.95880376422001556</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="4">
+        <v>13.12</v>
+      </c>
+      <c r="I22" s="4">
+        <v>72.680000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43617</v>
       </c>
@@ -868,8 +1034,14 @@
       <c r="G23">
         <v>0.44725194785326072</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="4">
+        <v>18.71</v>
+      </c>
+      <c r="I23" s="4">
+        <v>70.430000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43647</v>
       </c>
@@ -891,8 +1063,14 @@
       <c r="G24">
         <v>6.2361471592595849E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="4">
+        <v>15.08</v>
+      </c>
+      <c r="I24" s="4">
+        <v>55.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43678</v>
       </c>
@@ -914,8 +1092,14 @@
       <c r="G25">
         <v>0.70579391357463617</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="4">
+        <v>16.12</v>
+      </c>
+      <c r="I25" s="4">
+        <v>86.89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43709</v>
       </c>
@@ -937,8 +1121,14 @@
       <c r="G26">
         <v>0.51046067853253052</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="4">
+        <v>18.98</v>
+      </c>
+      <c r="I26" s="4">
+        <v>77.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43739</v>
       </c>
@@ -960,8 +1150,14 @@
       <c r="G27">
         <v>0.81236119936591367</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="4">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="I27" s="4">
+        <v>65.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43770</v>
       </c>
@@ -983,8 +1179,14 @@
       <c r="G28">
         <v>0.62815212540924792</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="4">
+        <v>13.22</v>
+      </c>
+      <c r="I28" s="4">
+        <v>56.57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43800</v>
       </c>
@@ -1006,8 +1208,14 @@
       <c r="G29">
         <v>1.5921292008214769</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="4">
+        <v>12.62</v>
+      </c>
+      <c r="I29" s="4">
+        <v>58.28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43831</v>
       </c>
@@ -1029,8 +1237,14 @@
       <c r="G30">
         <v>0.66190083656537702</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="4">
+        <v>13.78</v>
+      </c>
+      <c r="I30" s="4">
+        <v>72.98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43862</v>
       </c>
@@ -1052,8 +1266,14 @@
       <c r="G31">
         <v>3.387118366876344</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="4">
+        <v>18.84</v>
+      </c>
+      <c r="I31" s="4">
+        <v>109.67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43891</v>
       </c>
@@ -1075,8 +1295,14 @@
       <c r="G32">
         <v>0.78030699591151698</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="4">
+        <v>40.11</v>
+      </c>
+      <c r="I32" s="4">
+        <v>83.87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>43922</v>
       </c>
@@ -1098,8 +1324,14 @@
       <c r="G33">
         <v>-9.4575226559991663E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="4">
+        <v>53.54</v>
+      </c>
+      <c r="I33" s="4">
+        <v>53.59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>43952</v>
       </c>
@@ -1121,8 +1353,14 @@
       <c r="G34">
         <v>0.48015483072056359</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="4">
+        <v>34.15</v>
+      </c>
+      <c r="I34" s="4">
+        <v>51.55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43983</v>
       </c>
@@ -1144,8 +1382,14 @@
       <c r="G35">
         <v>0.36336360296791281</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="4">
+        <v>27.51</v>
+      </c>
+      <c r="I35" s="4">
+        <v>54.13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>44013</v>
       </c>
@@ -1167,8 +1411,14 @@
       <c r="G36">
         <v>0.63774288661647804</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="4">
+        <v>30.43</v>
+      </c>
+      <c r="I36" s="4">
+        <v>41.98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>44044</v>
       </c>
@@ -1190,8 +1440,14 @@
       <c r="G37">
         <v>1.7287633053973579</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="4">
+        <v>24.46</v>
+      </c>
+      <c r="I37" s="4">
+        <v>47.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>44075</v>
       </c>
@@ -1213,8 +1469,14 @@
       <c r="G38">
         <v>0.81737013204221531</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="4">
+        <v>26.41</v>
+      </c>
+      <c r="I38" s="4">
+        <v>39.21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>44105</v>
       </c>
@@ -1236,8 +1498,14 @@
       <c r="G39">
         <v>0.40465515504101801</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="4">
+        <v>26.37</v>
+      </c>
+      <c r="I39" s="4">
+        <v>61.91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>44136</v>
       </c>
@@ -1259,8 +1527,14 @@
       <c r="G40">
         <v>0.2006908060245565</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="4">
+        <v>38.020000000000003</v>
+      </c>
+      <c r="I40" s="4">
+        <v>40.840000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>44166</v>
       </c>
@@ -1282,8 +1556,14 @@
       <c r="G41">
         <v>0.6584713510560225</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="4">
+        <v>20.57</v>
+      </c>
+      <c r="I41" s="4">
+        <v>48.98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>44197</v>
       </c>
@@ -1305,8 +1585,14 @@
       <c r="G42">
         <v>0.73775990613938214</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="4">
+        <v>22.75</v>
+      </c>
+      <c r="I42" s="4">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>44228</v>
       </c>
@@ -1328,8 +1614,14 @@
       <c r="G43">
         <v>1.597578269986387</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="4">
+        <v>33.090000000000003</v>
+      </c>
+      <c r="I43" s="4">
+        <v>75.66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44256</v>
       </c>
@@ -1351,8 +1643,14 @@
       <c r="G44">
         <v>1.042133969392381</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="4">
+        <v>27.95</v>
+      </c>
+      <c r="I44" s="4">
+        <v>71.27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44287</v>
       </c>
@@ -1374,8 +1672,14 @@
       <c r="G45">
         <v>0.80294359179841102</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="4">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="I45" s="4">
+        <v>58.13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>44317</v>
       </c>
@@ -1397,8 +1701,14 @@
       <c r="G46">
         <v>1.7080709315477951</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="4">
+        <v>18.61</v>
+      </c>
+      <c r="I46" s="4">
+        <v>52.04</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>44348</v>
       </c>
@@ -1420,8 +1730,14 @@
       <c r="G47">
         <v>0.58548690962253747</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="4">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="I47" s="4">
+        <v>57.27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>44378</v>
       </c>
@@ -1443,8 +1759,14 @@
       <c r="G48">
         <v>1.1442300473160589</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="4">
+        <v>15.83</v>
+      </c>
+      <c r="I48" s="4">
+        <v>61.19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>44409</v>
       </c>
@@ -1466,8 +1788,14 @@
       <c r="G49">
         <v>0.95269023867037916</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="4">
+        <v>18.239999999999998</v>
+      </c>
+      <c r="I49" s="4">
+        <v>59.54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>44440</v>
       </c>
@@ -1489,8 +1817,14 @@
       <c r="G50">
         <v>1.07829177152692</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="4">
+        <v>16.48</v>
+      </c>
+      <c r="I50" s="4">
+        <v>61.07</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>44470</v>
       </c>
@@ -1512,8 +1846,14 @@
       <c r="G51">
         <v>0.66834971397419451</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="4">
+        <v>23.14</v>
+      </c>
+      <c r="I51" s="4">
+        <v>75.45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>44501</v>
       </c>
@@ -1535,8 +1875,14 @@
       <c r="G52">
         <v>1.2344199148499679</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="4">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="I52" s="4">
+        <v>84.04</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>44531</v>
       </c>
@@ -1558,8 +1904,14 @@
       <c r="G53">
         <v>0.65541051549392781</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="4">
+        <v>27.19</v>
+      </c>
+      <c r="I53" s="4">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>44562</v>
       </c>
@@ -1581,8 +1933,14 @@
       <c r="G54">
         <v>0.93245549203178124</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="4">
+        <v>17.22</v>
+      </c>
+      <c r="I54" s="4">
+        <v>85.14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>44593</v>
       </c>
@@ -1604,8 +1962,14 @@
       <c r="G55">
         <v>0.713903236891966</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="4">
+        <v>24.83</v>
+      </c>
+      <c r="I55" s="4">
+        <v>100.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>44621</v>
       </c>
@@ -1627,8 +1991,14 @@
       <c r="G56">
         <v>0.57085530133413664</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="4">
+        <v>30.15</v>
+      </c>
+      <c r="I56" s="4">
+        <v>106.88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>44652</v>
       </c>
@@ -1650,8 +2020,14 @@
       <c r="G57">
         <v>0.78556320849638861</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="4">
+        <v>20.56</v>
+      </c>
+      <c r="I57" s="4">
+        <v>128.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>44682</v>
       </c>
@@ -1673,8 +2049,14 @@
       <c r="G58">
         <v>1.4149425217580329</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="4">
+        <v>33.4</v>
+      </c>
+      <c r="I58" s="4">
+        <v>107.12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>44713</v>
       </c>
@@ -1696,8 +2078,14 @@
       <c r="G59">
         <v>0.65336229777322175</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="4">
+        <v>26.19</v>
+      </c>
+      <c r="I59" s="4">
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>44743</v>
       </c>
@@ -1719,8 +2107,14 @@
       <c r="G60">
         <v>0.7134602763039799</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="4">
+        <v>28.71</v>
+      </c>
+      <c r="I60" s="4">
+        <v>116.36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>44774</v>
       </c>
@@ -1742,8 +2136,14 @@
       <c r="G61">
         <v>0.6072620725962512</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="4">
+        <v>21.33</v>
+      </c>
+      <c r="I61" s="4">
+        <v>124.84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>44805</v>
       </c>
@@ -1765,8 +2165,14 @@
       <c r="G62">
         <v>1.0416240127568961</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="4">
+        <v>25.87</v>
+      </c>
+      <c r="I62" s="4">
+        <v>141.88999999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>44835</v>
       </c>
@@ -1788,8 +2194,14 @@
       <c r="G63">
         <v>0.66671792401072949</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="4">
+        <v>31.62</v>
+      </c>
+      <c r="I63" s="4">
+        <v>147.91999999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>44866</v>
       </c>
@@ -1811,8 +2223,14 @@
       <c r="G64">
         <v>1.992203679153091</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" s="4">
+        <v>25.88</v>
+      </c>
+      <c r="I64" s="4">
+        <v>127.27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>44896</v>
       </c>
@@ -1834,8 +2252,14 @@
       <c r="G65">
         <v>0.84549305695049026</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" s="4">
+        <v>20.58</v>
+      </c>
+      <c r="I65" s="4">
+        <v>121.61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>44927</v>
       </c>
@@ -1857,8 +2281,14 @@
       <c r="G66">
         <v>1.497785720407887</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" s="4">
+        <v>21.67</v>
+      </c>
+      <c r="I66" s="4">
+        <v>99.54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>44958</v>
       </c>
@@ -1880,8 +2310,14 @@
       <c r="G67">
         <v>0.91379915087974717</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67" s="4">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="I67" s="4">
+        <v>123.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>44986</v>
       </c>
@@ -1903,8 +2339,14 @@
       <c r="G68">
         <v>1.097500042427721</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68" s="4">
+        <v>20.7</v>
+      </c>
+      <c r="I68" s="4">
+        <v>135.93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>45017</v>
       </c>
@@ -1926,8 +2368,14 @@
       <c r="G69">
         <v>0.68547598864630199</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69" s="4">
+        <v>18.7</v>
+      </c>
+      <c r="I69" s="4">
+        <v>122.46</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>45047</v>
       </c>
@@ -1949,8 +2397,14 @@
       <c r="G70">
         <v>1.5035600105238831</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70" s="4">
+        <v>15.78</v>
+      </c>
+      <c r="I70" s="4">
+        <v>136.02000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>45078</v>
       </c>
@@ -1972,8 +2426,14 @@
       <c r="G71">
         <v>0.90945122167107684</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71" s="4">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="I71" s="4">
+        <v>110.64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>45108</v>
       </c>
@@ -1995,8 +2455,14 @@
       <c r="G72">
         <v>0.87878218176931155</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72" s="4">
+        <v>13.59</v>
+      </c>
+      <c r="I72" s="4">
+        <v>112.03</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>45139</v>
       </c>
@@ -2018,8 +2484,14 @@
       <c r="G73">
         <v>1.091249879391152</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73" s="4">
+        <v>13.63</v>
+      </c>
+      <c r="I73" s="4">
+        <v>107.93</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>45170</v>
       </c>
@@ -2041,8 +2513,14 @@
       <c r="G74">
         <v>1.090301645252828</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74" s="4">
+        <v>13.57</v>
+      </c>
+      <c r="I74" s="4">
+        <v>113.55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>45200</v>
       </c>
@@ -2064,8 +2542,14 @@
       <c r="G75">
         <v>0.9826132565782717</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75" s="4">
+        <v>17.52</v>
+      </c>
+      <c r="I75" s="4">
+        <v>126.86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>45231</v>
       </c>
@@ -2087,8 +2571,14 @@
       <c r="G76">
         <v>1.253878361503048</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76" s="4">
+        <v>18.14</v>
+      </c>
+      <c r="I76" s="4">
+        <v>115.32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>45261</v>
       </c>
@@ -2110,8 +2600,14 @@
       <c r="G77">
         <v>1.2614540610906451</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77" s="4">
+        <v>12.92</v>
+      </c>
+      <c r="I77" s="4">
+        <v>114.62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>45292</v>
       </c>
@@ -2133,8 +2629,14 @@
       <c r="G78">
         <v>1.0147271323864819</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78" s="4">
+        <v>12.45</v>
+      </c>
+      <c r="I78" s="4">
+        <v>107.28</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>45323</v>
       </c>
@@ -2156,8 +2658,14 @@
       <c r="G79">
         <v>1.0196012324709911</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79" s="4">
+        <v>14.35</v>
+      </c>
+      <c r="I79" s="4">
+        <v>109.1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>45352</v>
       </c>
@@ -2179,8 +2687,14 @@
       <c r="G80">
         <v>1.44738608879959</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" s="4">
+        <v>13.4</v>
+      </c>
+      <c r="I80" s="4">
+        <v>86.38</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>45383</v>
       </c>
@@ -2202,8 +2716,14 @@
       <c r="G81">
         <v>1.233584490977234</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="I81" s="4">
+        <v>107.46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>45413</v>
       </c>
@@ -2225,8 +2745,14 @@
       <c r="G82">
         <v>1.0522160156146569</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" s="4">
+        <v>15.65</v>
+      </c>
+      <c r="I82" s="4">
+        <v>91.14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>45444</v>
       </c>
@@ -2248,8 +2774,14 @@
       <c r="G83">
         <v>1.408944616056562</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" s="4">
+        <v>12.92</v>
+      </c>
+      <c r="I83" s="4">
+        <v>98.59</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>45474</v>
       </c>
@@ -2271,8 +2803,14 @@
       <c r="G84">
         <v>1.4839509653945691</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" s="4">
+        <v>12.44</v>
+      </c>
+      <c r="I84" s="4">
+        <v>99.41</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>45505</v>
       </c>
@@ -2294,8 +2832,14 @@
       <c r="G85">
         <v>1.134805133582302</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" s="4">
+        <v>16.36</v>
+      </c>
+      <c r="I85" s="4">
+        <v>107.77</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>45536</v>
       </c>
@@ -2317,8 +2861,14 @@
       <c r="G86">
         <v>0.8428892082532472</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" s="4">
+        <v>15</v>
+      </c>
+      <c r="I86" s="4">
+        <v>94.61</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>45566</v>
       </c>
@@ -2340,8 +2890,14 @@
       <c r="G87">
         <v>1.2987488945430219</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" s="4">
+        <v>16.73</v>
+      </c>
+      <c r="I87" s="4">
+        <v>135.18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>45597</v>
       </c>
@@ -2363,8 +2919,14 @@
       <c r="G88">
         <v>1.41556995626024</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" s="4">
+        <v>23.16</v>
+      </c>
+      <c r="I88" s="4">
+        <v>95.22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>45627</v>
       </c>
@@ -2386,8 +2948,14 @@
       <c r="G89">
         <v>0.9830613143721445</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" s="4">
+        <v>13.51</v>
+      </c>
+      <c r="I89" s="4">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>45658</v>
       </c>
@@ -2408,6 +2976,12 @@
       </c>
       <c r="G90">
         <v>0.87296742189159271</v>
+      </c>
+      <c r="H90" s="4">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="I90" s="4">
+        <v>91.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>